<commit_message>
remplire le JDT et faire le bilan
</commit_message>
<xml_diff>
--- a/JDT/Journal-de-Travail_SchertenleibRomain.xlsx
+++ b/JDT/Journal-de-Travail_SchertenleibRomain.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Docker\P_165-NoSQL\JDT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B26AABA3-49C4-49F6-AB05-F6E77E2C56E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D905A3F-41AC-4742-97BD-56E8E30162B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="56">
   <si>
     <t>Auteur:</t>
   </si>
@@ -185,6 +185,30 @@
   </si>
   <si>
     <t xml:space="preserve">remplire le journal de travail et faire les commits </t>
+  </si>
+  <si>
+    <t>documentation du le cache redis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">faire la partie 2 du projet </t>
+  </si>
+  <si>
+    <t xml:space="preserve">finire l'implementation du todoscontrolleur </t>
+  </si>
+  <si>
+    <t>corriger les erreurs de delete sur la partie 1</t>
+  </si>
+  <si>
+    <t>corriger les erreurs d'update sur la partie 1</t>
+  </si>
+  <si>
+    <t>corriger un point sur la partie 2 avec les utilisatueurs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">documentation du le cache redis et tester des bouts de code </t>
+  </si>
+  <si>
+    <t>commencer l'implémentation du cache redis</t>
   </si>
 </sst>
 </file>
@@ -1188,16 +1212,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>310</c:v>
+                  <c:v>590</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>85</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2121,16 +2145,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.20202020202020202</c:v>
+                  <c:v>0.15340909090909091</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.6262626262626263</c:v>
+                  <c:v>0.67045454545454541</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.17171717171717171</c:v>
+                  <c:v>0.17613636363636365</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -4317,9 +4341,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O532"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4374,7 +4398,7 @@
       <c r="B3" s="86"/>
       <c r="C3" s="67" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>8 heures 15 minutes</v>
+        <v>14 heures 40 minutes</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="3"/>
@@ -4389,15 +4413,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="17">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="D4" s="17">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>375</v>
+        <v>640</v>
       </c>
       <c r="E4" s="24">
         <f>SUM(C4:D4)</f>
-        <v>495</v>
+        <v>880</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4771,11 +4795,13 @@
       <c r="G20" s="39"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="63" t="str">
+      <c r="A21" s="63">
         <f>IF(ISBLANK(B21),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B21))</f>
-        <v/>
-      </c>
-      <c r="B21" s="34"/>
+        <v>19</v>
+      </c>
+      <c r="B21" s="34">
+        <v>45782</v>
+      </c>
       <c r="C21" s="35">
         <v>1</v>
       </c>
@@ -4791,11 +4817,13 @@
       <c r="G21" s="40"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="62" t="str">
+      <c r="A22" s="62">
         <f>IF(ISBLANK(B22),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B22))</f>
-        <v/>
-      </c>
-      <c r="B22" s="30"/>
+        <v>19</v>
+      </c>
+      <c r="B22" s="30">
+        <v>45782</v>
+      </c>
       <c r="C22" s="31"/>
       <c r="D22" s="32">
         <v>50</v>
@@ -4809,11 +4837,13 @@
       <c r="G22" s="39"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="63" t="str">
+      <c r="A23" s="63">
         <f>IF(ISBLANK(B23),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B23))</f>
-        <v/>
-      </c>
-      <c r="B23" s="34"/>
+        <v>19</v>
+      </c>
+      <c r="B23" s="34">
+        <v>45782</v>
+      </c>
       <c r="C23" s="35"/>
       <c r="D23" s="36">
         <v>25</v>
@@ -4827,11 +4857,13 @@
       <c r="G23" s="40"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="62" t="str">
+      <c r="A24" s="62">
         <f>IF(ISBLANK(B24),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B24))</f>
-        <v/>
-      </c>
-      <c r="B24" s="30"/>
+        <v>19</v>
+      </c>
+      <c r="B24" s="30">
+        <v>45782</v>
+      </c>
       <c r="C24" s="31"/>
       <c r="D24" s="32">
         <v>15</v>
@@ -4857,63 +4889,105 @@
       <c r="G25" s="40"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="62" t="str">
+      <c r="A26" s="62">
         <f>IF(ISBLANK(B26),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B26))</f>
-        <v/>
-      </c>
-      <c r="B26" s="30"/>
+        <v>20</v>
+      </c>
+      <c r="B26" s="30">
+        <v>45789</v>
+      </c>
       <c r="C26" s="31"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="23"/>
+      <c r="D26" s="32">
+        <v>10</v>
+      </c>
+      <c r="E26" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>43</v>
+      </c>
       <c r="G26" s="39"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="63" t="str">
+      <c r="A27" s="63">
         <f>IF(ISBLANK(B27),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B27))</f>
-        <v/>
-      </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="23"/>
+        <v>20</v>
+      </c>
+      <c r="B27" s="34">
+        <v>45789</v>
+      </c>
+      <c r="C27" s="35">
+        <v>1</v>
+      </c>
+      <c r="D27" s="36">
+        <v>30</v>
+      </c>
+      <c r="E27" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>49</v>
+      </c>
       <c r="G27" s="40"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="62" t="str">
+      <c r="A28" s="62">
         <f>IF(ISBLANK(B28),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B28))</f>
-        <v/>
-      </c>
-      <c r="B28" s="30"/>
+        <v>20</v>
+      </c>
+      <c r="B28" s="30">
+        <v>45789</v>
+      </c>
       <c r="C28" s="31"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="22"/>
+      <c r="D28" s="32">
+        <v>35</v>
+      </c>
+      <c r="E28" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="22" t="s">
+        <v>50</v>
+      </c>
       <c r="G28" s="39"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="63" t="str">
+      <c r="A29" s="63">
         <f>IF(ISBLANK(B29),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B29))</f>
-        <v/>
-      </c>
-      <c r="B29" s="34"/>
+        <v>20</v>
+      </c>
+      <c r="B29" s="34">
+        <v>45789</v>
+      </c>
       <c r="C29" s="35"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="22"/>
+      <c r="D29" s="36">
+        <v>25</v>
+      </c>
+      <c r="E29" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" s="22" t="s">
+        <v>48</v>
+      </c>
       <c r="G29" s="40"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="62" t="str">
+      <c r="A30" s="62">
         <f>IF(ISBLANK(B30),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B30))</f>
-        <v/>
-      </c>
-      <c r="B30" s="30"/>
+        <v>20</v>
+      </c>
+      <c r="B30" s="30">
+        <v>45789</v>
+      </c>
       <c r="C30" s="31"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="23"/>
+      <c r="D30" s="32">
+        <v>15</v>
+      </c>
+      <c r="E30" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="F30" s="23" t="s">
+        <v>47</v>
+      </c>
       <c r="G30" s="39"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -4929,75 +5003,123 @@
       <c r="G31" s="40"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="62" t="str">
+      <c r="A32" s="62">
         <f>IF(ISBLANK(B32),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B32))</f>
-        <v/>
-      </c>
-      <c r="B32" s="30"/>
+        <v>21</v>
+      </c>
+      <c r="B32" s="30">
+        <v>45796</v>
+      </c>
       <c r="C32" s="31"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="23"/>
+      <c r="D32" s="32">
+        <v>10</v>
+      </c>
+      <c r="E32" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="F32" s="23" t="s">
+        <v>43</v>
+      </c>
       <c r="G32" s="39"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="63" t="str">
+      <c r="A33" s="63">
         <f>IF(ISBLANK(B33),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B33))</f>
-        <v/>
-      </c>
-      <c r="B33" s="34"/>
-      <c r="C33" s="35"/>
+        <v>21</v>
+      </c>
+      <c r="B33" s="34">
+        <v>45796</v>
+      </c>
+      <c r="C33" s="35">
+        <v>1</v>
+      </c>
       <c r="D33" s="36"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="22"/>
+      <c r="E33" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" s="22" t="s">
+        <v>51</v>
+      </c>
       <c r="G33" s="40"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="62" t="str">
+      <c r="A34" s="62">
         <f>IF(ISBLANK(B34),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B34))</f>
-        <v/>
-      </c>
-      <c r="B34" s="30"/>
+        <v>21</v>
+      </c>
+      <c r="B34" s="30">
+        <v>45796</v>
+      </c>
       <c r="C34" s="31"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="22"/>
+      <c r="D34" s="32">
+        <v>30</v>
+      </c>
+      <c r="E34" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" s="22" t="s">
+        <v>52</v>
+      </c>
       <c r="G34" s="39"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="63" t="str">
+      <c r="A35" s="63">
         <f>IF(ISBLANK(B35),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B35))</f>
-        <v/>
-      </c>
-      <c r="B35" s="34"/>
+        <v>21</v>
+      </c>
+      <c r="B35" s="34">
+        <v>45796</v>
+      </c>
       <c r="C35" s="35"/>
-      <c r="D35" s="36"/>
-      <c r="E35" s="37"/>
-      <c r="F35" s="23"/>
+      <c r="D35" s="36">
+        <v>35</v>
+      </c>
+      <c r="E35" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" s="23" t="s">
+        <v>53</v>
+      </c>
       <c r="G35" s="40"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="62" t="str">
+      <c r="A36" s="62">
         <f>IF(ISBLANK(B36),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B36))</f>
-        <v/>
-      </c>
-      <c r="B36" s="30"/>
+        <v>21</v>
+      </c>
+      <c r="B36" s="30">
+        <v>45796</v>
+      </c>
       <c r="C36" s="31"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="22"/>
+      <c r="D36" s="32">
+        <v>45</v>
+      </c>
+      <c r="E36" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F36" s="22" t="s">
+        <v>54</v>
+      </c>
       <c r="G36" s="39"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="63" t="str">
+      <c r="A37" s="63">
         <f>IF(ISBLANK(B37),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B37))</f>
-        <v/>
-      </c>
-      <c r="B37" s="34"/>
+        <v>21</v>
+      </c>
+      <c r="B37" s="34">
+        <v>45796</v>
+      </c>
       <c r="C37" s="35"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="37"/>
-      <c r="F37" s="22"/>
+      <c r="D37" s="36">
+        <v>30</v>
+      </c>
+      <c r="E37" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F37" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="G37" s="40"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -11083,11 +11205,11 @@
       </c>
       <c r="B6">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E6,'Journal de travail'!$D$7:$D$532)</f>
-        <v>100</v>
+        <v>135</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:C10" si="0">SUM(A6:B6)</f>
-        <v>100</v>
+        <v>135</v>
       </c>
       <c r="E6" s="70" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11095,11 +11217,11 @@
       </c>
       <c r="F6" s="71" t="str">
         <f>QUOTIENT(SUM(A6:B6),60)&amp;" h "&amp;TEXT(MOD(SUM(A6:B6),60), "00")&amp;" min"</f>
-        <v>1 h 40 min</v>
+        <v>2 h 15 min</v>
       </c>
       <c r="G6" s="72">
         <f>SUM(A6:B6)/$C$11</f>
-        <v>0.20202020202020202</v>
+        <v>0.15340909090909091</v>
       </c>
       <c r="L6" s="51" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11116,15 +11238,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>190</v>
+        <v>350</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>310</v>
+        <v>590</v>
       </c>
       <c r="E7" s="73" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11132,11 +11254,11 @@
       </c>
       <c r="F7" s="74" t="str">
         <f t="shared" ref="F7:F11" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>5 h 10 min</v>
+        <v>9 h 50 min</v>
       </c>
       <c r="G7" s="75">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$11</f>
-        <v>0.6262626262626263</v>
+        <v>0.67045454545454541</v>
       </c>
       <c r="L7" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11194,11 +11316,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>85</v>
+        <v>155</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>85</v>
+        <v>155</v>
       </c>
       <c r="E9" s="77" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11206,11 +11328,11 @@
       </c>
       <c r="F9" s="74" t="str">
         <f t="shared" si="1"/>
-        <v>1 h 25 min</v>
+        <v>2 h 35 min</v>
       </c>
       <c r="G9" s="75">
         <f t="shared" si="2"/>
-        <v>0.17171717171717171</v>
+        <v>0.17613636363636365</v>
       </c>
       <c r="L9" s="55" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11262,26 +11384,26 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>SUM(A6:A10)</f>
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="B11">
         <f>SUM(B6:B10)</f>
-        <v>375</v>
+        <v>640</v>
       </c>
       <c r="C11">
         <f>SUM(A11:B11)</f>
-        <v>495</v>
+        <v>880</v>
       </c>
       <c r="E11" s="81" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="71" t="str">
         <f t="shared" si="1"/>
-        <v>8 h 15 min</v>
+        <v>14 h 40 min</v>
       </c>
       <c r="G11" s="82">
         <f>C11/C12</f>
-        <v>9.375E-2</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="L11" s="56" t="s">
         <v>18</v>
@@ -11325,26 +11447,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010080C9F2488912074FB587B9AD9ADAE5BB" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="dfbaf9a740889adeb1cda0be194d08b7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xmlns:ns3="eefa3612-053e-497a-ae76-8a76877f5e22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4f25723b2930dbb90e2332f0c8c46e31" ns2:_="" ns3:_="">
     <xsd:import namespace="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
@@ -11545,10 +11647,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7F8341A-4C75-4689-8311-30F611A1EC8F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
+    <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -11567,20 +11700,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7F8341A-4C75-4689-8311-30F611A1EC8F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
-    <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>